<commit_message>
Update 2005 data (fix Grande-Anse indexing)
This commit moves an incorrectly placed index in the tax base data from 2005 (which was transcribed from the GNB PDF) from a Grand Manan subdistrict to Grande-Anse, fixing a bug in the data processing pipeline.
</commit_message>
<xml_diff>
--- a/data/data_raw/2005/GNB2005_tax_base.xlsx
+++ b/data/data_raw/2005/GNB2005_tax_base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luismbvarona/GitHub/nb-service-prices-and-tax-rates/data/data_raw/2005/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF83B6C6-D4E9-3F43-AFC5-D5D56CFF73F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEAD9A9-B40D-E543-8958-83F73CB867CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4269,9 +4269,6 @@
       <c r="P64" s="1"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="B65" s="1" t="s">
         <v>390</v>
       </c>
@@ -4313,7 +4310,9 @@
       <c r="P65" s="1"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="B66" s="1" t="s">
         <v>238</v>
       </c>

</xml_diff>

<commit_message>
Update 2005 data (fix Grande-Anse indexing) (#1)
This commit moves an incorrectly placed index in the tax base data from 2005 (which was transcribed from the GNB PDF) from a Grand Manan subdistrict to Grande-Anse, fixing a bug in the data processing pipeline.
</commit_message>
<xml_diff>
--- a/data/data_raw/2005/GNB2005_tax_base.xlsx
+++ b/data/data_raw/2005/GNB2005_tax_base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luismbvarona/GitHub/nb-service-prices-and-tax-rates/data/data_raw/2005/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF83B6C6-D4E9-3F43-AFC5-D5D56CFF73F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEAD9A9-B40D-E543-8958-83F73CB867CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4269,9 +4269,6 @@
       <c r="P64" s="1"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="B65" s="1" t="s">
         <v>390</v>
       </c>
@@ -4313,7 +4310,9 @@
       <c r="P65" s="1"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="B66" s="1" t="s">
         <v>238</v>
       </c>

</xml_diff>